<commit_message>
test real robot traj v1
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_2_.xlsx
+++ b/dynamics/src/dynamics/tested_state_traj/tested_robot_traj_2_.xlsx
@@ -423,122 +423,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.202886707818579</v>
+        <v>0.2028864896758006</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.01986466890848812</v>
+        <v>0.002539495620456482</v>
       </c>
       <c r="C1" t="n">
-        <v>1.376669968070769</v>
+        <v>1.379316785363834</v>
       </c>
       <c r="D1" t="n">
-        <v>0.2139908537329471</v>
+        <v>0.188939888900502</v>
       </c>
       <c r="E1" t="n">
-        <v>1.570796379327078</v>
+        <v>1.570796384046431</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.367909666075958</v>
+        <v>-1.367909888287239</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2483787665506595</v>
+        <v>0.2484977296296271</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.01986772926019229</v>
+        <v>0.002377709119405816</v>
       </c>
       <c r="C2" t="n">
-        <v>1.376688281609331</v>
+        <v>1.380518500463224</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2139756031505863</v>
+        <v>0.1878999627744357</v>
       </c>
       <c r="E2" t="n">
-        <v>1.570796379392748</v>
+        <v>1.570796384423863</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.322417608204078</v>
+        <v>-1.322298649847111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.4522133501513073</v>
+        <v>0.4528663241188721</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.01988144166478938</v>
+        <v>0.001652798332930176</v>
       </c>
       <c r="C3" t="n">
-        <v>1.376770338403657</v>
+        <v>1.385902980825687</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2139072704307262</v>
+        <v>0.1832404042758736</v>
       </c>
       <c r="E3" t="n">
-        <v>1.57079637968699</v>
+        <v>1.570796386115009</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.118583028457701</v>
+        <v>-1.117930062140237</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.7389892563021565</v>
+        <v>0.7403935328885739</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.01990073371613993</v>
+        <v>0.0006329176826605036</v>
       </c>
       <c r="C4" t="n">
-        <v>1.376885784522431</v>
+        <v>1.393478433468806</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2138111327816999</v>
+        <v>0.1766848478679089</v>
       </c>
       <c r="E4" t="n">
-        <v>1.570796380100961</v>
+        <v>1.570796388494291</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.8318071277294455</v>
+        <v>-0.8304028629126882</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.9428238399028049</v>
+        <v>0.9447621273778194</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.01991444612073703</v>
+        <v>-9.199310381513776e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>1.376967841316757</v>
+        <v>1.398862913831269</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2137428000618398</v>
+        <v>0.1720252893693467</v>
       </c>
       <c r="E5" t="n">
-        <v>1.570796380395203</v>
+        <v>1.570796390185437</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.627972547983068</v>
+        <v>-0.6260342752058142</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.9883158986348846</v>
+        <v>0.9903733673316449</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.01991750647244119</v>
+        <v>-0.0002537796048658041</v>
       </c>
       <c r="C6" t="n">
-        <v>1.376986154855319</v>
+        <v>1.40006462893066</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2137275494794789</v>
+        <v>0.1709853632432805</v>
       </c>
       <c r="E6" t="n">
-        <v>1.570796380460873</v>
+        <v>1.570796390562869</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.5824804901111889</v>
+        <v>-0.5804230367656862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>